<commit_message>
Ultimos cambios para la primera version de resolucion
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteArqueo.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteArqueo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Empeños\Comprobantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Empe-o\Empeño.WindowsForms\bin\Debug\Empeños\Comprobantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3492" windowWidth="28800" windowHeight="15456"/>
+    <workbookView xWindow="0" yWindow="3948" windowWidth="28800" windowHeight="15456"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Cédula:</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Total en Proróga :</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -218,28 +221,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -248,8 +257,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,10 +544,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,75 +558,75 @@
     <col min="4" max="4" width="67.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:8" ht="64.95" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A2" s="16" t="s">
+    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" ht="64.95" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A5" s="16" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A7" s="16" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="A7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:8" ht="52.2" customHeight="1" x14ac:dyDescent="0.95">
+    <row r="9" spans="1:4" ht="52.2" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.95">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,7 +634,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.95">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -633,192 +642,207 @@
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" ht="330" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="A14" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A13" s="4" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-    </row>
-    <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A17" s="12" t="s">
+    <row r="16" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A19" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A19" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
     </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A20" s="8" t="s">
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A21" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A21" s="8" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A22" s="8" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A23" s="8" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A25" s="8"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A26" s="14" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A28" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-    </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A29" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>6</v>
-      </c>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
     </row>
-    <row r="31" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-    </row>
-    <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A32" s="11" t="s">
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="A31" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+    </row>
+    <row r="33" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="A34" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A32:D32"/>
+  <mergeCells count="26">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A30:D31"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A13:D13"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A32:D33"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="21" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Version 1.2.3 Oficial Instalada en Grecia
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteArqueo.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteArqueo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Empe-o\Empeño.WindowsForms\bin\Debug\Empeños\Comprobantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3948" windowWidth="28800" windowHeight="15456"/>
+    <workbookView xWindow="0" yWindow="4845" windowWidth="28800" windowHeight="15450"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Cédula:</t>
   </si>
@@ -44,9 +44,6 @@
     <t>GRACIAS</t>
   </si>
   <si>
-    <t>Favor conserve éste recibo para poder retirar su empeño y para que realice los pagos de intereses.</t>
-  </si>
-  <si>
     <t>Jorge Arce Gonzalez</t>
   </si>
   <si>
@@ -102,6 +99,33 @@
   </si>
   <si>
     <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Favor conserve éste comprobante para constar la revisión del Arqueo.</t>
+  </si>
+  <si>
+    <r>
+      <t>Yo,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> {Empleado} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="48"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>hago constar que los datos mostrados en este reporte son veridicos y me comprometo a responder por lo que en el esta descrito.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -112,7 +136,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +164,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -231,6 +262,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -247,6 +284,9 @@
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -544,279 +584,311 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.44140625" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
     <col min="2" max="2" width="99" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" customWidth="1"/>
-    <col min="4" max="4" width="67.88671875" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4" ht="64.95" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A2" s="17" t="s">
+    <row r="1" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A3" s="17" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:4" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:4" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A5" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A6" s="17" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-    </row>
-    <row r="7" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
-      <c r="A7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-    </row>
-    <row r="8" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.95">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="52.2" customHeight="1" x14ac:dyDescent="0.95">
+    <row r="9" spans="1:4" ht="52.15" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+    </row>
+    <row r="10" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.95">
+    <row r="12" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" ht="330" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A14" s="21" t="s">
+    <row r="13" spans="1:4" ht="330" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A14" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A20" s="12" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.95">
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
       <c r="A22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-    </row>
-    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A23" s="8" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-    </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A24" s="8" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-    </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A25" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-    </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A28" s="15" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A33" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.95">
-      <c r="A31" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-    </row>
-    <row r="32" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="1:4" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
     </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.95">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+    </row>
+    <row r="36" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A36" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="1:4" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+    </row>
+    <row r="39" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="A39" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="27">
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:D7"/>
@@ -832,17 +904,18 @@
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A39:D39"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A32:D33"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A37:D38"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A27:D30"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="21" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios finales de la 1.4.11
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteArqueo.xlsx
+++ b/Empeño.WindowsForms/Empeños/Comprobantes/ComprobanteArqueo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtjarquinm\Documents\GitHub-Donovan\Empe-o\Empeño.WindowsForms\Empeños\Comprobantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D70925-54B1-46D4-910C-9488123C8069}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4845" windowWidth="28800" windowHeight="15450"/>
+    <workbookView xWindow="-21720" yWindow="525" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Cédula:</t>
   </si>
@@ -105,7 +106,7 @@
   </si>
   <si>
     <r>
-      <t>Yo,</t>
+      <t>Yo, __________________________________</t>
     </r>
     <r>
       <rPr>
@@ -115,7 +116,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> {Empleado} </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -124,17 +125,20 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>hago constar que los datos mostrados en este reporte son veridicos y me comprometo a responder por lo que en el esta descrito.</t>
+      <t>hago constar que los datos mostrados en este reporte son veridicos y me hago responsable por los bienes custodiados.</t>
     </r>
+  </si>
+  <si>
+    <t>Administrador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -225,7 +229,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -240,7 +244,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -261,17 +265,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,26 +298,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -580,101 +584,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D30"/>
+      <selection activeCell="A42" sqref="A42:D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.453125" customWidth="1"/>
     <col min="2" max="2" width="99" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="67.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.81640625" customWidth="1"/>
+    <col min="4" max="4" width="67.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="19" t="s">
+    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:4" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="19" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:4" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" ht="121.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A5" s="19" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="19" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="19" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" ht="54.65" customHeight="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="52.15" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" ht="52.15" customHeight="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-    </row>
-    <row r="10" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -682,7 +686,7 @@
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -690,21 +694,21 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" ht="330" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-    </row>
-    <row r="14" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A14" s="24" t="s">
+    <row r="13" spans="1:4" ht="330" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -718,177 +722,218 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A19" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A20" s="14" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A21" s="14" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-    </row>
-    <row r="25" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-    </row>
-    <row r="26" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+    <row r="27" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-    </row>
-    <row r="30" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+    </row>
+    <row r="28" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:8" ht="59.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="59.25" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A33" s="17" t="s">
+    <row r="33" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A33" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-    </row>
-    <row r="34" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-    </row>
-    <row r="36" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A36" s="17" t="s">
+    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+    </row>
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A36" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-    </row>
-    <row r="37" spans="1:4" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+    </row>
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+    </row>
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A39" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+    </row>
+    <row r="40" spans="1:4" ht="153.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-    </row>
-    <row r="38" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-    </row>
-    <row r="39" spans="1:4" ht="59.25" x14ac:dyDescent="0.75">
-      <c r="A39" s="16" t="s">
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+    </row>
+    <row r="41" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="1.1499999999999999">
+      <c r="A42" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="29">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A40:D41"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A27:D30"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A7:D7"/>
@@ -897,25 +942,6 @@
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A37:D38"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A27:D30"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="21" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>